<commit_message>
update table acronyms areas
</commit_message>
<xml_diff>
--- a/Output_figures/Table 3.xlsx
+++ b/Output_figures/Table 3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B338"/>
+  <dimension ref="A1:B327"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -928,3518 +928,3430 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CB-unassigned</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr"/>
+          <t>CEA</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Central amygdalar nucleus</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CEA</t>
+          <t>CENT</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Central amygdalar nucleus</t>
+          <t>Central lobule</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CENT</t>
+          <t>CL</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Central lobule</t>
+          <t>Central lateral nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CL</t>
+          <t>CLA</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Central lateral nucleus of the thalamus</t>
+          <t>Claustrum</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>CLA</t>
+          <t>CLI</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Claustrum</t>
+          <t>Central linear nucleus raphe</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CLI</t>
+          <t>CM</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Central linear nucleus raphe</t>
+          <t>Central medial nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>CM</t>
+          <t>COAa</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Central medial nucleus of the thalamus</t>
+          <t>Cortical amygdalar area, anterior part</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>COAa</t>
+          <t>COAp</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Cortical amygdalar area, anterior part</t>
+          <t>Cortical amygdalar area, posterior part</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>COAp</t>
+          <t>COPY</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Cortical amygdalar area, posterior part</t>
+          <t>Copula pyramidis</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>COPY</t>
+          <t>CP</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Copula pyramidis</t>
+          <t>Caudoputamen</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CP</t>
+          <t>CS</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Caudoputamen</t>
+          <t>Superior central nucleus raphe</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>CTXsp</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Superior central nucleus raphe</t>
+          <t>Cortical subplate</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>CTXsp</t>
+          <t>CU</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Cortical subplate</t>
+          <t>Cuneate nucleus</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>CTXsp-unassigned</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
+          <t>CUL</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Culmen</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>CU</t>
+          <t>CUN</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Cuneate nucleus</t>
+          <t>Cuneiform nucleus</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CUL</t>
+          <t>DCO</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Culmen</t>
+          <t>Dorsal cochlear nucleus</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>CUN</t>
+          <t>DEC</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Cuneiform nucleus</t>
+          <t>Declive (VI)</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>DCO</t>
+          <t>DG</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Dorsal cochlear nucleus</t>
+          <t>Dentate gyrus</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>DEC</t>
+          <t>DMH</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Declive (VI)</t>
+          <t>Dorsomedial nucleus of the hypothalamus</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>DG</t>
+          <t>DMX</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Dentate gyrus</t>
+          <t>Dorsal motor nucleus of the vagus nerve</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>DMH</t>
+          <t>DN</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Dorsomedial nucleus of the hypothalamus</t>
+          <t>Dentate nucleus</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>DMX</t>
+          <t>DP</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Dorsal motor nucleus of the vagus nerve</t>
+          <t>Dorsal peduncular area</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>DN</t>
+          <t>DR</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Dentate nucleus</t>
+          <t>Dorsal nucleus raphe</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>DP</t>
+          <t>DT</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Dorsal peduncular area</t>
+          <t>Dorsal terminal nucleus of the accessory optic tract</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>DR</t>
+          <t>DTN</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Dorsal nucleus raphe</t>
+          <t>Dorsal tegmental nucleus</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>DT</t>
+          <t>ECT</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Dorsal terminal nucleus of the accessory optic tract</t>
+          <t>Ectorhinal area</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>DTN</t>
+          <t>ECU</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Dorsal tegmental nucleus</t>
+          <t>External cuneate nucleus</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>ECT</t>
+          <t>ENTl</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Ectorhinal area</t>
+          <t>Entorhinal area, lateral part</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>ECU</t>
+          <t>ENTm</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>External cuneate nucleus</t>
+          <t>Entorhinal area, medial part, dorsal zone</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>ENTl</t>
+          <t>EPd</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Entorhinal area, lateral part</t>
+          <t>Endopiriform nucleus, dorsal part</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>ENTm</t>
+          <t>EPv</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Entorhinal area, medial part, dorsal zone</t>
+          <t>Endopiriform nucleus, ventral part</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>EPd</t>
+          <t>EW</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Endopiriform nucleus, dorsal part</t>
+          <t>Edinger-Westphal nucleus</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>EPv</t>
+          <t>Eth</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Endopiriform nucleus, ventral part</t>
+          <t>Ethmoid nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>EW</t>
+          <t>FC</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Edinger-Westphal nucleus</t>
+          <t>Fasciola cinerea</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Eth</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Ethmoid nucleus of the thalamus</t>
+          <t>Flocculus</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>FC</t>
+          <t>FN</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Fasciola cinerea</t>
+          <t>Fastigial nucleus</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>FL</t>
+          <t>FOTU</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Flocculus</t>
+          <t>Folium-tuber vermis (VII)</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>FN</t>
+          <t>FRP</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Fastigial nucleus</t>
+          <t>Frontal pole, cerebral cortex</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>FOTU</t>
+          <t>FS</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Folium-tuber vermis (VII)</t>
+          <t>Fundus of striatum</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>FRP</t>
+          <t>GPe</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Frontal pole, cerebral cortex</t>
+          <t>Globus pallidus, external segment</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>FS</t>
+          <t>GPi</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Fundus of striatum</t>
+          <t>Globus pallidus, internal segment</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>GPe</t>
+          <t>GR</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Globus pallidus, external segment</t>
+          <t>Gracile nucleus</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>GPi</t>
+          <t>GRN</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Globus pallidus, internal segment</t>
+          <t>Gigantocellular reticular nucleus</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>GR</t>
+          <t>GU</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Gracile nucleus</t>
+          <t>Gustatory areas</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>GRN</t>
+          <t>HATA</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Gigantocellular reticular nucleus</t>
+          <t>Hippocampo-amygdalar transition area</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>GU</t>
+          <t>HPF</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Gustatory areas</t>
+          <t>Hippocampal formation</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>HATA</t>
+          <t>HY</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Hippocampo-amygdalar transition area</t>
+          <t>Hypothalamus</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>HPF</t>
+          <t>I5</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Hippocampal formation</t>
+          <t>Intertrigeminal nucleus</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>HPF-unassigned</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr"/>
+          <t>IA</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Intercalated amygdalar nucleus</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>HY</t>
+          <t>IAD</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Hypothalamus</t>
+          <t>Interanterodorsal nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>HY-unassigned</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr"/>
+          <t>IAM</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Interanteromedial nucleus of the thalamus</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>I5</t>
+          <t>IC</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Intertrigeminal nucleus</t>
+          <t>Inferior colliculus</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>IA</t>
+          <t>ICB</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Intercalated amygdalar nucleus</t>
+          <t>Infracerebellar nucleus</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>IAD</t>
+          <t>IF</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Interanterodorsal nucleus of the thalamus</t>
+          <t>Interfascicular nucleus raphe</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>IAM</t>
+          <t>IG</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Interanteromedial nucleus of the thalamus</t>
+          <t>Induseum griseum</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>IC</t>
+          <t>IGL</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Inferior colliculus</t>
+          <t>Intergeniculate leaflet of the lateral geniculate complex</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>ICB</t>
+          <t>III</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Infracerebellar nucleus</t>
+          <t>Oculomotor nucleus</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>IF</t>
+          <t>ILA</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Interfascicular nucleus raphe</t>
+          <t>Infralimbic area</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>IG</t>
+          <t>IMD</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Induseum griseum</t>
+          <t>Intermediodorsal nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>IGL</t>
+          <t>IO</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Intergeniculate leaflet of the lateral geniculate complex</t>
+          <t>Inferior olivary complex</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>III</t>
+          <t>IP</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Oculomotor nucleus</t>
+          <t>Interposed nucleus</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>ILA</t>
+          <t>IPN</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Infralimbic area</t>
+          <t>Interpeduncular nucleus</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>IMD</t>
+          <t>IRN</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Intermediodorsal nucleus of the thalamus</t>
+          <t>Intermediate reticular nucleus</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>IO</t>
+          <t>ISN</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Inferior olivary complex</t>
+          <t>Inferior salivatory nucleus</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>IP</t>
+          <t>IV</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Interposed nucleus</t>
+          <t>Trochlear nucleus</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>IPN</t>
+          <t>IntG</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Interpeduncular nucleus</t>
+          <t>Intermediate geniculate nucleus</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>IRN</t>
+          <t>Isocortex</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Intermediate reticular nucleus</t>
+          <t>Isocortex</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>ISN</t>
+          <t>LA</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Inferior salivatory nucleus</t>
+          <t>Lateral amygdalar nucleus</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>IV</t>
+          <t>LAV</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Trochlear nucleus</t>
+          <t>Lateral vestibular nucleus</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>IntG</t>
+          <t>LC</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Intermediate geniculate nucleus</t>
+          <t>Locus ceruleus</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Isocortex</t>
+          <t>LD</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Isocortex</t>
+          <t>Lateral dorsal nucleus of thalamus</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>LA</t>
+          <t>LDT</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Lateral amygdalar nucleus</t>
+          <t>Laterodorsal tegmental nucleus</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>LAV</t>
+          <t>LGd</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Lateral vestibular nucleus</t>
+          <t>Dorsal part of the lateral geniculate complex</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>LC</t>
+          <t>LGv</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Locus ceruleus</t>
+          <t>Ventral part of the lateral geniculate complex</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>LD</t>
+          <t>LH</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Lateral dorsal nucleus of thalamus</t>
+          <t>Lateral habenula</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>LDT</t>
+          <t>LHA</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Laterodorsal tegmental nucleus</t>
+          <t>Lateral hypothalamic area</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>LGd</t>
+          <t>LIN</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Dorsal part of the lateral geniculate complex</t>
+          <t>Linear nucleus of the medulla</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>LGv</t>
+          <t>LING</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Ventral part of the lateral geniculate complex</t>
+          <t>Lingula (I)</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>LH</t>
+          <t>LM</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Lateral habenula</t>
+          <t>Lateral mammillary nucleus</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>LHA</t>
+          <t>LP</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Lateral hypothalamic area</t>
+          <t>Lateral posterior nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>LIN</t>
+          <t>LPO</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Linear nucleus of the medulla</t>
+          <t>Lateral preoptic area</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>LING</t>
+          <t>LRN</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Lingula (I)</t>
+          <t>Lateral reticular nucleus</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>LM</t>
+          <t>LSc</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Lateral mammillary nucleus</t>
+          <t>Lateral septal nucleus, caudal (caudodorsal) part</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>LSr</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Lateral posterior nucleus of the thalamus</t>
+          <t>Lateral septal nucleus, rostral (rostroventral) part</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>LPO</t>
+          <t>LSv</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Lateral preoptic area</t>
+          <t>Lateral septal nucleus, ventral part</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>LRN</t>
+          <t>LT</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Lateral reticular nucleus</t>
+          <t>Lateral terminal nucleus of the accessory optic tract</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>LSc</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Lateral septal nucleus, caudal (caudodorsal) part</t>
+          <t>Magnocellular nucleus</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>LSr</t>
+          <t>MA3</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Lateral septal nucleus, rostral (rostroventral) part</t>
+          <t>Medial accesory oculomotor nucleus</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>LSv</t>
+          <t>MARN</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Lateral septal nucleus, ventral part</t>
+          <t>Magnocellular reticular nucleus</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>LT</t>
+          <t>MB</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Lateral terminal nucleus of the accessory optic tract</t>
+          <t>Midbrain</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>MD</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Magnocellular nucleus</t>
+          <t>Mediodorsal nucleus of thalamus</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>MA3</t>
+          <t>MDRN</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Medial accesory oculomotor nucleus</t>
+          <t>Medullary reticular nucleus</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>MARN</t>
+          <t>ME</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Magnocellular reticular nucleus</t>
+          <t>Median eminence</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>MB</t>
+          <t>MEA</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Midbrain</t>
+          <t>Medial amygdalar nucleus</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>MB-unassigned</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr"/>
+          <t>MEPO</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Median preoptic nucleus</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>MD</t>
+          <t>MG</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Mediodorsal nucleus of thalamus</t>
+          <t>Medial geniculate complex</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>MDRN</t>
+          <t>MH</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Medullary reticular nucleus</t>
+          <t>Medial habenula</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>ME</t>
+          <t>MM</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Median eminence</t>
+          <t>Medial mammillary nucleus</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>MEA</t>
+          <t>MOB</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Medial amygdalar nucleus</t>
+          <t>Main olfactory bulb</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>MEPO</t>
+          <t>MOp</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Median preoptic nucleus</t>
+          <t>Primary motor area</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>MG</t>
+          <t>MOs</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Medial geniculate complex</t>
+          <t>Secondary motor area</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>MH</t>
+          <t>MPN</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Medial habenula</t>
+          <t>Medial preoptic nucleus</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>MM</t>
+          <t>MPO</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Medial mammillary nucleus</t>
+          <t>Medial preoptic area</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>MOB</t>
+          <t>MPT</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Main olfactory bulb</t>
+          <t>Medial pretectal area</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>MOp</t>
+          <t>MRN</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Primary motor area</t>
+          <t>Midbrain reticular nucleus</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>MOs</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Secondary motor area</t>
+          <t>Medial septal nucleus</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>MPN</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Medial preoptic nucleus</t>
+          <t>Medial terminal nucleus of the accessory optic tract</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>MPO</t>
+          <t>MV</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Medial preoptic area</t>
+          <t>Medial vestibular nucleus</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>MPT</t>
+          <t>MY</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Medial pretectal area</t>
+          <t>Medulla</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>MRN</t>
+          <t>NB</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Midbrain reticular nucleus</t>
+          <t>Nucleus of the brachium of the inferior colliculus</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>NDB</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Medial septal nucleus</t>
+          <t>Diagonal band nucleus</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>NI</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Medial terminal nucleus of the accessory optic tract</t>
+          <t>Nucleus incertus</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>MV</t>
+          <t>NLL</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Medial vestibular nucleus</t>
+          <t>Nucleus of the lateral lemniscus</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>MY</t>
+          <t>NLOT</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Medulla</t>
+          <t>Nucleus of the lateral olfactory tract</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>MY-unassigned</t>
-        </is>
-      </c>
-      <c r="B156" t="inlineStr"/>
+          <t>NOD</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Nodulus (X)</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>NB</t>
+          <t>NOT</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Nucleus of the brachium of the inferior colliculus</t>
+          <t>Nucleus of the optic tract</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>NDB</t>
+          <t>NPC</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Diagonal band nucleus</t>
+          <t>Nucleus of the posterior commissure</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>NI</t>
+          <t>NR</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Nucleus incertus</t>
+          <t>Nucleus of Roller</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>NLL</t>
+          <t>NTB</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Nucleus of the lateral lemniscus</t>
+          <t>Nucleus of the trapezoid body</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>NLOT</t>
+          <t>NTS</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Nucleus of the lateral olfactory tract</t>
+          <t>Nucleus of the solitary tract</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>NOD</t>
+          <t>OLF</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Nodulus (X)</t>
+          <t>Olfactory areas</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>NOT</t>
+          <t>OP</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Nucleus of the optic tract</t>
+          <t>Olivary pretectal nucleus</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>NPC</t>
+          <t>ORBl</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Nucleus of the posterior commissure</t>
+          <t>Orbital area, lateral part</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>NR</t>
+          <t>ORBm</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Nucleus of Roller</t>
+          <t>Orbital area, medial part</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>NTB</t>
+          <t>ORBvl</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Nucleus of the trapezoid body</t>
+          <t>Orbital area, ventrolateral part</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>NTS</t>
+          <t>OT</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Nucleus of the solitary tract</t>
+          <t>Olfactory tubercle</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>OLF</t>
+          <t>OV</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Olfactory areas</t>
+          <t>Vascular organ of the lamina terminalis</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>OLF-unassigned</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr"/>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Pons</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>OP</t>
+          <t>P5</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Olivary pretectal nucleus</t>
+          <t>Peritrigeminal zone</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>ORBl</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Orbital area, lateral part</t>
+          <t>Posterior amygdalar nucleus</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>ORBm</t>
+          <t>PAA</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Orbital area, medial part</t>
+          <t>Piriform-amygdalar area</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>ORBvl</t>
+          <t>PAG</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Orbital area, ventrolateral part</t>
+          <t>Periaqueductal gray</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>OT</t>
+          <t>PAL</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Olfactory tubercle</t>
+          <t>Pallidum</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>OV</t>
+          <t>PAR</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Vascular organ of the lamina terminalis</t>
+          <t>Parasubiculum</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>PARN</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Pons</t>
+          <t>Parvicellular reticular nucleus</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>P-unassigned</t>
-        </is>
-      </c>
-      <c r="B177" t="inlineStr"/>
+          <t>PAS</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Parasolitary nucleus</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>P5</t>
+          <t>PB</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Peritrigeminal zone</t>
+          <t>Parabrachial nucleus</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>PBG</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Posterior amygdalar nucleus</t>
+          <t>Parabigeminal nucleus</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>PAA</t>
+          <t>PC5</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Piriform-amygdalar area</t>
+          <t>Parvicellular motor 5 nucleus</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>PAG</t>
+          <t>PCG</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Periaqueductal gray</t>
+          <t>Pontine central gray</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>PAL</t>
+          <t>PCN</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Pallidum</t>
+          <t>Paracentral nucleus</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>PAL-unassigned</t>
-        </is>
-      </c>
-      <c r="B183" t="inlineStr"/>
+          <t>PD</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>Posterodorsal preoptic nucleus</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>PAR</t>
+          <t>PDTg</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Parasubiculum</t>
+          <t>Posterodorsal tegmental nucleus</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>PARN</t>
+          <t>PERI</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Parvicellular reticular nucleus</t>
+          <t>Perirhinal area</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>PAS</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Parasolitary nucleus</t>
+          <t>Parafascicular nucleus</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>PB</t>
+          <t>PFL</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Parabrachial nucleus</t>
+          <t>Paraflocculus</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>PBG</t>
+          <t>PG</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Parabigeminal nucleus</t>
+          <t>Pontine gray</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>PC5</t>
+          <t>PGRNd</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Parvicellular motor 5 nucleus</t>
+          <t>Paragigantocellular reticular nucleus, dorsal part</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>PCG</t>
+          <t>PGRNl</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Pontine central gray</t>
+          <t>Paragigantocellular reticular nucleus, lateral part</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>PCN</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Paracentral nucleus</t>
+          <t>Posterior hypothalamic nucleus</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>PD</t>
+          <t>PIL</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Posterodorsal preoptic nucleus</t>
+          <t>Posterior intralaminar thalamic nucleus</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>PDTg</t>
+          <t>PIR</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Posterodorsal tegmental nucleus</t>
+          <t>Piriform area</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>PERI</t>
+          <t>PL</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Perirhinal area</t>
+          <t>Prelimbic area</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PMd</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Parafascicular nucleus</t>
+          <t>Dorsal premammillary nucleus</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>PFL</t>
+          <t>PMv</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Paraflocculus</t>
+          <t>Ventral premammillary nucleus</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>PG</t>
+          <t>PN</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Pontine gray</t>
+          <t>Paranigral nucleus</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>PGRNd</t>
+          <t>PO</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Paragigantocellular reticular nucleus, dorsal part</t>
+          <t>Posterior complex of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>PGRNl</t>
+          <t>POL</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Paragigantocellular reticular nucleus, lateral part</t>
+          <t>Posterior limiting nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>PH</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Posterior hypothalamic nucleus</t>
+          <t>Postsubiculum</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>PIL</t>
+          <t>PP</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Posterior intralaminar thalamic nucleus</t>
+          <t>Peripeduncular nucleus</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>PIR</t>
+          <t>PPN</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Piriform area</t>
+          <t>Pedunculopontine nucleus</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>PL</t>
+          <t>PPT</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Prelimbic area</t>
+          <t>Posterior pretectal nucleus</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>PMd</t>
+          <t>PPY</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Dorsal premammillary nucleus</t>
+          <t>Parapyramidal nucleus</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>PMv</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Ventral premammillary nucleus</t>
+          <t>Perireunensis nucleus</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>PN</t>
+          <t>PRE</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Paranigral nucleus</t>
+          <t>Presubiculum</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>PO</t>
+          <t>PRM</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Posterior complex of the thalamus</t>
+          <t>Paramedian lobule</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>POL</t>
+          <t>PRNc</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Posterior limiting nucleus of the thalamus</t>
+          <t>Pontine reticular nucleus, caudal part</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>PRNr</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Postsubiculum</t>
+          <t>Pontine reticular nucleus</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>PP</t>
+          <t>PRP</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Peripeduncular nucleus</t>
+          <t>Nucleus prepositus</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>PPN</t>
+          <t>PS</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Pedunculopontine nucleus</t>
+          <t>Parastrial nucleus</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>PST</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Posterior pretectal nucleus</t>
+          <t>Preparasubthalamic nucleus</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>PPY</t>
+          <t>PSTN</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Parapyramidal nucleus</t>
+          <t>Parasubthalamic nucleus</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>PSV</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Perireunensis nucleus</t>
+          <t>Principal sensory nucleus of the trigeminal</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>PRE</t>
+          <t>PT</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Presubiculum</t>
+          <t>Parataenial nucleus</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>PRM</t>
+          <t>PVH</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Paramedian lobule</t>
+          <t>Paraventricular hypothalamic nucleus</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>PRNc</t>
+          <t>PVHd</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Pontine reticular nucleus, caudal part</t>
+          <t>Paraventricular hypothalamic nucleus, descending division</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>PRNr</t>
+          <t>PVT</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Pontine reticular nucleus</t>
+          <t>Paraventricular nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>PRP</t>
+          <t>PVa</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Nucleus prepositus</t>
+          <t>Periventricular hypothalamic nucleus, anterior part</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>PS</t>
+          <t>PVi</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Parastrial nucleus</t>
+          <t>Periventricular hypothalamic nucleus, intermediate part</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>PST</t>
+          <t>PVp</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Preparasubthalamic nucleus</t>
+          <t>Periventricular hypothalamic nucleus, posterior part</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>PSTN</t>
+          <t>PVpo</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Parasubthalamic nucleus</t>
+          <t>Periventricular hypothalamic nucleus, preoptic part</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>PSV</t>
+          <t>PYR</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Principal sensory nucleus of the trigeminal</t>
+          <t>Pyramus (VIII)</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>Pa4</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Parataenial nucleus</t>
+          <t>Paratrochlear nucleus</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>PVH</t>
+          <t>Pa5</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Paraventricular hypothalamic nucleus</t>
+          <t>Paratrigeminal nucleus</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>PVHd</t>
+          <t>PeF</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Paraventricular hypothalamic nucleus, descending division</t>
+          <t>Perifornical nucleus</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>PVT</t>
+          <t>PoT</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Paraventricular nucleus of the thalamus</t>
+          <t>Posterior triangular thalamic nucleus</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>PVa</t>
+          <t>ProS</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Periventricular hypothalamic nucleus, anterior part</t>
+          <t>Prosubiculum</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>PVi</t>
+          <t>RCH</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Periventricular hypothalamic nucleus, intermediate part</t>
+          <t>Retrochiasmatic area</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>PVp</t>
+          <t>RE</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Periventricular hypothalamic nucleus, posterior part</t>
+          <t>Nucleus of reuniens</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>PVpo</t>
+          <t>RH</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Periventricular hypothalamic nucleus, preoptic part</t>
+          <t>Rhomboid nucleus</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>PYR</t>
+          <t>RL</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Pyramus (VIII)</t>
+          <t>Rostral linear nucleus raphe</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Pa4</t>
+          <t>RM</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Paratrochlear nucleus</t>
+          <t>Nucleus raphe magnus</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Pa5</t>
+          <t>RN</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Paratrigeminal nucleus</t>
+          <t>Red nucleus</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>PeF</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Perifornical nucleus</t>
+          <t>Nucleus raphe obscurus</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>PoT</t>
+          <t>RPA</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Posterior triangular thalamic nucleus</t>
+          <t>Nucleus raphe pallidus</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>ProS</t>
+          <t>RPF</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Prosubiculum</t>
+          <t>Retroparafascicular nucleus</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>RCH</t>
+          <t>RPO</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Retrochiasmatic area</t>
+          <t>Nucleus raphe pontis</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>RE</t>
+          <t>RR</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Nucleus of reuniens</t>
+          <t>Midbrain reticular nucleus, retrorubral area</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>RH</t>
+          <t>RSPagl</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Rhomboid nucleus</t>
+          <t>Retrosplenial area, lateral agranular part</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>RL</t>
+          <t>RSPd</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Rostral linear nucleus raphe</t>
+          <t>Retrosplenial area, dorsal part</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>RM</t>
+          <t>RSPv</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Nucleus raphe magnus</t>
+          <t>Retrosplenial area, ventral part</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>RN</t>
+          <t>RT</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Red nucleus</t>
+          <t>Reticular nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>SAG</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Nucleus raphe obscurus</t>
+          <t>Nucleus sagulum</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>RPA</t>
+          <t>SBPV</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Nucleus raphe pallidus</t>
+          <t>Subparaventricular zone</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>RPF</t>
+          <t>SCH</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Retroparafascicular nucleus</t>
+          <t>Suprachiasmatic nucleus</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>RPO</t>
+          <t>SCO</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Nucleus raphe pontis</t>
+          <t>Subcommissural organ</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>RR</t>
+          <t>SCm</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Midbrain reticular nucleus, retrorubral area</t>
+          <t>Superior colliculus, motor related</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>RSPagl</t>
+          <t>SCs</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Retrosplenial area, lateral agranular part</t>
+          <t>Superior colliculus, sensory related</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>RSPd</t>
+          <t>SF</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Retrosplenial area, dorsal part</t>
+          <t>Septofimbrial nucleus</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>RSPv</t>
+          <t>SFO</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Retrosplenial area, ventral part</t>
+          <t>Subfornical organ</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>RT</t>
+          <t>SG</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Reticular nucleus of the thalamus</t>
+          <t>Supragenual nucleus</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>SAG</t>
+          <t>SGN</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Nucleus sagulum</t>
+          <t>Suprageniculate nucleus</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>SBPV</t>
+          <t>SH</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Subparaventricular zone</t>
+          <t>Septohippocampal nucleus</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>SCH</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Suprachiasmatic nucleus</t>
+          <t>Substantia innominata</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>SCO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Subcommissural organ</t>
+          <t>Simple lobule</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>SCm</t>
+          <t>SLC</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Superior colliculus, motor related</t>
+          <t>Subceruleus nucleus</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>SCs</t>
+          <t>SLD</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Superior colliculus, sensory related</t>
+          <t>Sublaterodorsal nucleus</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>SF</t>
+          <t>SMT</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Septofimbrial nucleus</t>
+          <t>Submedial nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>SFO</t>
+          <t>SNc</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Subfornical organ</t>
+          <t>Substantia nigra, compact part</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>SG</t>
+          <t>SNr</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Supragenual nucleus</t>
+          <t>Substantia nigra, reticular part</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>SGN</t>
+          <t>SO</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Suprageniculate nucleus</t>
+          <t>Supraoptic nucleus</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>SH</t>
+          <t>SOC</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Septohippocampal nucleus</t>
+          <t>Superior olivary complex</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>SPA</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Substantia innominata</t>
+          <t>Subparafascicular area</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>SPFm</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Simple lobule</t>
+          <t>Subparafascicular nucleus, magnocellular part</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>SLC</t>
+          <t>SPFp</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>Subceruleus nucleus</t>
+          <t>Subparafascicular nucleus, parvicellular part</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>SLD</t>
+          <t>SPIV</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>Sublaterodorsal nucleus</t>
+          <t>Spinal vestibular nucleus</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>SMT</t>
+          <t>SPVC</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>Submedial nucleus of the thalamus</t>
+          <t>Spinal nucleus of the trigeminal, caudal part</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>SNc</t>
+          <t>SPVI</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>Substantia nigra, compact part</t>
+          <t>Spinal nucleus of the trigeminal, interpolar part</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>SNr</t>
+          <t>SPVO</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>Substantia nigra, reticular part</t>
+          <t>Spinal nucleus of the trigeminal, oral part</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>SO</t>
+          <t>SSp-bfd</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>Supraoptic nucleus</t>
+          <t>Primary somatosensory area, barrel field</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>SOC</t>
+          <t>SSp-ll</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>Superior olivary complex</t>
+          <t>Primary somatosensory area, lower limb</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>SPA</t>
+          <t>SSp-m</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>Subparafascicular area</t>
+          <t>Primary somatosensory area, mouth</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>SPFm</t>
+          <t>SSp-n</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>Subparafascicular nucleus, magnocellular part</t>
+          <t>Primary somatosensory area, nose</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>SPFp</t>
+          <t>SSp-tr</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>Subparafascicular nucleus, parvicellular part</t>
+          <t>Primary somatosensory area, trunk</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>SPIV</t>
+          <t>SSp-ul</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>Spinal vestibular nucleus</t>
+          <t>Primary somatosensory area, upper limb</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>SPVC</t>
+          <t>SSp-un</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>Spinal nucleus of the trigeminal, caudal part</t>
+          <t>Primary somatosensory area, unassigned</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>SPVI</t>
+          <t>SSs</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>Spinal nucleus of the trigeminal, interpolar part</t>
+          <t>Supplemental somatosensory area</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>SPVO</t>
+          <t>STN</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>Spinal nucleus of the trigeminal, oral part</t>
+          <t>Subthalamic nucleus</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>SSp-bfd</t>
+          <t>STR</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>Primary somatosensory area, barrel field</t>
+          <t>Striatum</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>SSp-ll</t>
+          <t>SUB</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>Primary somatosensory area, lower limb</t>
+          <t>Subiculum</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>SSp-m</t>
+          <t>SUM</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>Primary somatosensory area, mouth</t>
+          <t>Supramammillary nucleus</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>SSp-n</t>
+          <t>SUT</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>Primary somatosensory area, nose</t>
+          <t>Supratrigeminal nucleus</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>SSp-tr</t>
+          <t>SUV</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>Primary somatosensory area, trunk</t>
+          <t>Superior vestibular nucleus</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>SSp-ul</t>
+          <t>SubG</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>Primary somatosensory area, upper limb</t>
+          <t>Subgeniculate nucleus</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>SSp-un</t>
+          <t>TEa</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>Primary somatosensory area, unassigned</t>
+          <t>Temporal association areas</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>SSs</t>
+          <t>TH</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>Supplemental somatosensory area</t>
+          <t>Thalamus</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>STN</t>
+          <t>TMd</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>Subthalamic nucleus</t>
+          <t>Tuberomammillary nucleus, dorsal part</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>STR</t>
+          <t>TMv</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>Striatum</t>
+          <t>Tuberomammillary nucleus, ventral part</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>STR-unassigned</t>
-        </is>
-      </c>
-      <c r="B290" t="inlineStr"/>
+          <t>TR</t>
+        </is>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Postpiriform transition area</t>
+        </is>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>SUB</t>
+          <t>TRN</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>Subiculum</t>
+          <t>Tegmental reticular nucleus</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>SUM</t>
+          <t>TRS</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>Supramammillary nucleus</t>
+          <t>Triangular nucleus of septum</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>SUT</t>
+          <t>TT</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>Supratrigeminal nucleus</t>
+          <t>Taenia tecta</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>SUV</t>
+          <t>TU</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>Superior vestibular nucleus</t>
+          <t>Tuberal nucleus</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>SubG</t>
+          <t>UVU</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>Subgeniculate nucleus</t>
+          <t>Uvula (IX)</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>TEa</t>
+          <t>V</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>Temporal association areas</t>
+          <t>Motor nucleus of trigeminal</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>TH</t>
+          <t>VAL</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>Thalamus</t>
+          <t>Ventral anterior-lateral complex of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>TH-unassigned</t>
-        </is>
-      </c>
-      <c r="B298" t="inlineStr"/>
+          <t>VCO</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Ventral cochlear nucleus</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>TMd</t>
+          <t>VI</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>Tuberomammillary nucleus, dorsal part</t>
+          <t>Abducens nucleus</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>TMv</t>
+          <t>VII</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>Tuberomammillary nucleus, ventral part</t>
+          <t>Facial motor nucleus</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>TR</t>
+          <t>VISC</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>Postpiriform transition area</t>
+          <t>Visceral area</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>TRN</t>
+          <t>VISa</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>Tegmental reticular nucleus</t>
+          <t>Anterior area</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>TRS</t>
+          <t>VISal</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>Triangular nucleus of septum</t>
+          <t>Anterolateral visual area</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>TT</t>
+          <t>VISam</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>Taenia tecta</t>
+          <t>Anteromedial visual area</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>TU</t>
+          <t>VISl</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>Tuberal nucleus</t>
+          <t>Lateral visual area</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>UVU</t>
+          <t>VISli</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>Uvula (IX)</t>
+          <t>Laterointermediate area</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>VISp</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>Motor nucleus of trigeminal</t>
+          <t>Primary visual area</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>VAL</t>
+          <t>VISpl</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>Ventral anterior-lateral complex of the thalamus</t>
+          <t>Posterolateral visual area</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>VCO</t>
+          <t>VISpm</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>Ventral cochlear nucleus</t>
+          <t>posteromedial visual area</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>VI</t>
+          <t>VISpor</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>Abducens nucleus</t>
+          <t>Postrhinal area</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>VII</t>
+          <t>VISrl</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>Facial motor nucleus</t>
+          <t>Rostrolateral visual area</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>VISC</t>
+          <t>VLPO</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>Visceral area</t>
+          <t>Ventrolateral preoptic nucleus</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>VISa</t>
+          <t>VM</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>Anterior area</t>
+          <t>Ventral medial nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>VISal</t>
+          <t>VMH</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>Anterolateral visual area</t>
+          <t>Ventromedial hypothalamic nucleus</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>VISam</t>
+          <t>VMPO</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>Anteromedial visual area</t>
+          <t>Ventromedial preoptic nucleus</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>VISl</t>
+          <t>VPL</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>Lateral visual area</t>
+          <t>Ventral posterolateral nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>VISli</t>
+          <t>VPLpc</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Laterointermediate area</t>
+          <t>Ventral posterolateral nucleus of the thalamus, parvicellular part</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>VISp</t>
+          <t>VPM</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Primary visual area</t>
+          <t>Ventral posteromedial nucleus of the thalamus</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>VISpl</t>
+          <t>VPMpc</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>Posterolateral visual area</t>
+          <t>Ventral posteromedial nucleus of the thalamus, parvicellular part</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>VISpm</t>
+          <t>VTA</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>posteromedial visual area</t>
+          <t>Ventral tegmental area</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>VISpor</t>
+          <t>VTN</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>Postrhinal area</t>
+          <t>Ventral tegmental nucleus</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>VISrl</t>
+          <t>VeCB</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>Rostrolateral visual area</t>
+          <t>Vestibulocerebellar nucleus</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>VLPO</t>
+          <t>XII</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>Ventrolateral preoptic nucleus</t>
+          <t>Hypoglossal nucleus</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>VM</t>
+          <t>Xi</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>Ventral medial nucleus of the thalamus</t>
+          <t>Xiphoid thalamic nucleus</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>VMH</t>
+          <t>ZI</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>Ventromedial hypothalamic nucleus</t>
+          <t>Zona incerta</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>VMPO</t>
+          <t>x</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>Ventromedial preoptic nucleus</t>
+          <t>Nucleus x</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>VPL</t>
+          <t>y</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
-        <is>
-          <t>Ventral posterolateral nucleus of the thalamus</t>
-        </is>
-      </c>
-    </row>
-    <row r="328">
-      <c r="A328" t="inlineStr">
-        <is>
-          <t>VPLpc</t>
-        </is>
-      </c>
-      <c r="B328" t="inlineStr">
-        <is>
-          <t>Ventral posterolateral nucleus of the thalamus, parvicellular part</t>
-        </is>
-      </c>
-    </row>
-    <row r="329">
-      <c r="A329" t="inlineStr">
-        <is>
-          <t>VPM</t>
-        </is>
-      </c>
-      <c r="B329" t="inlineStr">
-        <is>
-          <t>Ventral posteromedial nucleus of the thalamus</t>
-        </is>
-      </c>
-    </row>
-    <row r="330">
-      <c r="A330" t="inlineStr">
-        <is>
-          <t>VPMpc</t>
-        </is>
-      </c>
-      <c r="B330" t="inlineStr">
-        <is>
-          <t>Ventral posteromedial nucleus of the thalamus, parvicellular part</t>
-        </is>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331" t="inlineStr">
-        <is>
-          <t>VTA</t>
-        </is>
-      </c>
-      <c r="B331" t="inlineStr">
-        <is>
-          <t>Ventral tegmental area</t>
-        </is>
-      </c>
-    </row>
-    <row r="332">
-      <c r="A332" t="inlineStr">
-        <is>
-          <t>VTN</t>
-        </is>
-      </c>
-      <c r="B332" t="inlineStr">
-        <is>
-          <t>Ventral tegmental nucleus</t>
-        </is>
-      </c>
-    </row>
-    <row r="333">
-      <c r="A333" t="inlineStr">
-        <is>
-          <t>VeCB</t>
-        </is>
-      </c>
-      <c r="B333" t="inlineStr">
-        <is>
-          <t>Vestibulocerebellar nucleus</t>
-        </is>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334" t="inlineStr">
-        <is>
-          <t>XII</t>
-        </is>
-      </c>
-      <c r="B334" t="inlineStr">
-        <is>
-          <t>Hypoglossal nucleus</t>
-        </is>
-      </c>
-    </row>
-    <row r="335">
-      <c r="A335" t="inlineStr">
-        <is>
-          <t>Xi</t>
-        </is>
-      </c>
-      <c r="B335" t="inlineStr">
-        <is>
-          <t>Xiphoid thalamic nucleus</t>
-        </is>
-      </c>
-    </row>
-    <row r="336">
-      <c r="A336" t="inlineStr">
-        <is>
-          <t>ZI</t>
-        </is>
-      </c>
-      <c r="B336" t="inlineStr">
-        <is>
-          <t>Zona incerta</t>
-        </is>
-      </c>
-    </row>
-    <row r="337">
-      <c r="A337" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="B337" t="inlineStr">
-        <is>
-          <t>Nucleus x</t>
-        </is>
-      </c>
-    </row>
-    <row r="338">
-      <c r="A338" t="inlineStr">
-        <is>
-          <t>y</t>
-        </is>
-      </c>
-      <c r="B338" t="inlineStr">
         <is>
           <t>Nucleus y</t>
         </is>

</xml_diff>